<commit_message>
Data preparation and score prediction
</commit_message>
<xml_diff>
--- a/Excel/words explaination.xlsx
+++ b/Excel/words explaination.xlsx
@@ -425,13 +425,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="1" max="1" width="29.453125" customWidth="1"/>
+    <col min="2" max="2" width="29.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>